<commit_message>
Ajuste final de enceramento
</commit_message>
<xml_diff>
--- a/Documentação final do projeto/Estrategia de validação.xlsx
+++ b/Documentação final do projeto/Estrategia de validação.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador.IMDPOA\Documents\GitHub\TCC\Documentação final do projeto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
   </bookViews>
@@ -20,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$3:$A$18</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +30,7 @@
     <author>NEIMAR MOISES GOBBI</author>
   </authors>
   <commentList>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -92,19 +87,7 @@
     <t xml:space="preserve">Nome </t>
   </si>
   <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Marciano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rodrigo </t>
-  </si>
-  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Fabricio</t>
   </si>
   <si>
     <t>Praticidade?</t>
@@ -243,11 +226,23 @@
   <si>
     <t>Relevância</t>
   </si>
+  <si>
+    <t>Rodrigo (Coordenador)</t>
+  </si>
+  <si>
+    <t>Marciano (Professor)</t>
+  </si>
+  <si>
+    <t>Fabricio (Professor)</t>
+  </si>
+  <si>
+    <t>Bruno (Professor)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,6 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,7 +433,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +451,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -532,7 +527,7 @@
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-9802-4A9B-A754-BB43199BF209}"/>
               </c:ext>
@@ -553,7 +548,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -576,7 +571,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -599,7 +594,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -622,7 +617,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -655,7 +650,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -702,7 +697,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-9802-4A9B-A754-BB43199BF209}"/>
             </c:ext>
@@ -718,12 +713,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1970106272"/>
-        <c:axId val="-1970108992"/>
+        <c:axId val="57651712"/>
+        <c:axId val="20862016"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1970106272"/>
+        <c:axId val="57651712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +738,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1970108992"/>
+        <c:crossAx val="20862016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1970108992"/>
+        <c:axId val="20862016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1970106272"/>
+        <c:crossAx val="57651712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -804,7 +799,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -822,6 +817,7 @@
       <c:rotX val="15"/>
       <c:rotY val="20"/>
       <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -867,7 +863,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -890,7 +886,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -913,7 +909,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -936,7 +932,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -959,7 +955,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -992,7 +988,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1045,7 +1041,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-8294-46F9-AECB-DC41E028BDC1}"/>
             </c:ext>
@@ -1061,12 +1057,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1970108448"/>
-        <c:axId val="-1970117152"/>
+        <c:axId val="57653248"/>
+        <c:axId val="82209600"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1970108448"/>
+        <c:axId val="57653248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +1086,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1970117152"/>
+        <c:crossAx val="82209600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1098,7 +1094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1970117152"/>
+        <c:axId val="82209600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1970108448"/>
+        <c:crossAx val="57653248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1166,7 +1162,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1219,7 +1215,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-4877-4EA0-880F-C622069EB2C2}"/>
@@ -1240,7 +1236,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-4877-4EA0-880F-C622069EB2C2}"/>
@@ -1261,7 +1257,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-4877-4EA0-880F-C622069EB2C2}"/>
@@ -1282,7 +1278,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1294,16 +1290,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Rodrigo </c:v>
+                  <c:v>Rodrigo (Coordenador)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Bruno</c:v>
+                  <c:v>Bruno (Professor)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Marciano</c:v>
+                  <c:v>Marciano (Professor)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Fabricio</c:v>
+                  <c:v>Fabricio (Professor)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1327,7 +1323,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-4877-4EA0-880F-C622069EB2C2}"/>
             </c:ext>
@@ -1341,12 +1337,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1970116608"/>
-        <c:axId val="-1970107360"/>
+        <c:axId val="58544128"/>
+        <c:axId val="82211328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1970116608"/>
+        <c:axId val="58544128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1363,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1970107360"/>
+        <c:crossAx val="82211328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1374,7 +1371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1970107360"/>
+        <c:axId val="82211328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,7 +1396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1970116608"/>
+        <c:crossAx val="58544128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1899,7 +1896,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1934,7 +1931,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2111,7 +2108,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2122,7 +2119,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,19 +2148,19 @@
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="25"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="26"/>
       <c r="F2" s="16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H2" s="20"/>
     </row>
@@ -2172,30 +2169,30 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -2216,13 +2213,13 @@
         <v>5</v>
       </c>
       <c r="H4" s="21">
-        <f t="shared" ref="H4:H7" si="0">SUM(B4:G4)/6</f>
+        <f t="shared" ref="H4:H5" si="0">SUM(B4:G4)/6</f>
         <v>4.833333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -2279,7 +2276,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -2314,7 +2311,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="18">
-        <f t="shared" ref="C8:H8" si="1">SUM(C4:C7)</f>
+        <f t="shared" ref="C8:G8" si="1">SUM(C4:C7)</f>
         <v>18</v>
       </c>
       <c r="D8" s="18">
@@ -2337,25 +2334,25 @@
         <f>SUM(B8:G8)/6</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="25">
         <f>I6-I7</f>
         <v>1.5599999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="27">
+        <v>24</v>
+      </c>
+      <c r="B9" s="28">
         <f>((B8+C8)/2)/4</f>
         <v>4.25</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28">
         <f>((D8+E8)/2)/4</f>
         <v>4</v>
       </c>
-      <c r="E9" s="27"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="19">
         <f>F8/4</f>
         <v>4.25</v>
@@ -2378,10 +2375,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2391,7 +2388,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="12">
         <v>1</v>
@@ -2404,7 +2401,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" s="8">
         <v>2</v>
@@ -2417,7 +2414,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" s="8">
         <v>3</v>
@@ -2430,7 +2427,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" s="8">
         <v>4</v>
@@ -2443,7 +2440,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="8">
         <v>5</v>
@@ -2456,37 +2453,37 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>